<commit_message>
more progress on video downloads and metadata
</commit_message>
<xml_diff>
--- a/ben-build tools/old video catalog/vimeo-table.xlsx
+++ b/ben-build tools/old video catalog/vimeo-table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/XCode/projects/Publish Web Sites/theskinny/ben-build tools/old video catalog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{81861613-CA4B-364C-9288-434AACC860CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6061940-2A63-4844-A821-D3251E6593B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="6440" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="4260" yWindow="3280" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vimeo-table" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="233">
   <si>
     <t>Privacy</t>
   </si>
@@ -714,13 +714,22 @@
   </si>
   <si>
     <t>Home Movies (V &amp; K) 2014</t>
+  </si>
+  <si>
+    <t>Home Movies (V &amp; K):  September 2012 - December 2013</t>
+  </si>
+  <si>
+    <t>Home Movies (V &amp; K):  January - August, 2012</t>
+  </si>
+  <si>
+    <t>Family Videos from Russia 2012</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -874,6 +883,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1221,7 +1237,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1244,6 +1260,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1599,12 +1619,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D117" sqref="D1:D1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1672,7 +1692,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>112</v>
       </c>
@@ -1682,9 +1702,14 @@
       <c r="C5" s="6">
         <v>40891.337500000001</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D5" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>67</v>
       </c>
@@ -1694,7 +1719,12 @@
       <c r="C6" s="6">
         <v>41520.818749999999</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E6" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -1792,7 +1822,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
@@ -1802,7 +1832,12 @@
       <c r="C15" s="6">
         <v>41273.538194444445</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E15" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -1816,7 +1851,7 @@
       </c>
       <c r="D16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>110</v>
       </c>
@@ -1826,9 +1861,14 @@
       <c r="C17" s="6">
         <v>40891.344444444447</v>
       </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="D17" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E17" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>63</v>
       </c>
@@ -1838,9 +1878,14 @@
       <c r="C18" s="6">
         <v>41568.683333333334</v>
       </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D18" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E18" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>66</v>
       </c>
@@ -1850,7 +1895,12 @@
       <c r="C19" s="6">
         <v>41520.866666666669</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E19" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
@@ -1900,7 +1950,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>200</v>
       </c>
@@ -1958,7 +2008,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>97</v>
       </c>
@@ -1968,9 +2018,14 @@
       <c r="C28" s="6">
         <v>41024.543749999997</v>
       </c>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>1818656</v>
+      </c>
+      <c r="E28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>39</v>
       </c>
@@ -2016,7 +2071,7 @@
       </c>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>105</v>
       </c>
@@ -2026,7 +2081,12 @@
       <c r="C32" s="6">
         <v>40935.612500000003</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32">
+        <v>1818656</v>
+      </c>
+      <c r="E32" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
@@ -2093,7 +2153,7 @@
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>80</v>
       </c>
@@ -2103,7 +2163,12 @@
       <c r="C38" s="6">
         <v>41199.600694444445</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E38" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
@@ -2189,7 +2254,7 @@
       </c>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>68</v>
       </c>
@@ -2199,7 +2264,12 @@
       <c r="C46" s="6">
         <v>41515.78125</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E46" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
@@ -2218,7 +2288,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>16</v>
       </c>
@@ -2252,7 +2322,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>38</v>
       </c>
@@ -2293,7 +2363,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>92</v>
       </c>
@@ -2303,7 +2373,12 @@
       <c r="C53" s="6">
         <v>41059.445833333331</v>
       </c>
-      <c r="D53" s="3"/>
+      <c r="D53">
+        <v>1818656</v>
+      </c>
+      <c r="E53" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -2334,7 +2409,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>108</v>
       </c>
@@ -2344,9 +2419,14 @@
       <c r="C56" s="6">
         <v>40898.02847222222</v>
       </c>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D56" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E56" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>55</v>
       </c>
@@ -2486,7 +2566,7 @@
       </c>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>48</v>
       </c>
@@ -2532,7 +2612,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>177</v>
       </c>
@@ -2544,7 +2624,7 @@
       </c>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>181</v>
       </c>
@@ -2573,7 +2653,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>116</v>
       </c>
@@ -2583,9 +2663,14 @@
       <c r="C73" s="6">
         <v>40886.065972222219</v>
       </c>
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D73" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E73" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>98</v>
       </c>
@@ -2595,9 +2680,14 @@
       <c r="C74" s="6">
         <v>41012.455555555556</v>
       </c>
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D74">
+        <v>1818656</v>
+      </c>
+      <c r="E74" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>107</v>
       </c>
@@ -2607,9 +2697,14 @@
       <c r="C75" s="6">
         <v>40898.040972222225</v>
       </c>
-      <c r="D75" s="3"/>
-    </row>
-    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D75" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E75" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>47</v>
       </c>
@@ -2638,7 +2733,7 @@
       </c>
       <c r="D77" s="3"/>
     </row>
-    <row r="78" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>183</v>
       </c>
@@ -2662,7 +2757,7 @@
       </c>
       <c r="D79" s="3"/>
     </row>
-    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>51</v>
       </c>
@@ -2679,7 +2774,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>53</v>
       </c>
@@ -2696,7 +2791,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>57</v>
       </c>
@@ -2737,7 +2832,7 @@
       </c>
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>75</v>
       </c>
@@ -2747,9 +2842,14 @@
       <c r="C85" s="6">
         <v>41271.511111111111</v>
       </c>
-      <c r="D85" s="3"/>
-    </row>
-    <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D85" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E85" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>122</v>
       </c>
@@ -2759,9 +2859,14 @@
       <c r="C86" s="6">
         <v>40841.902777777781</v>
       </c>
-      <c r="D86" s="3"/>
-    </row>
-    <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D86" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E86" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>121</v>
       </c>
@@ -2771,9 +2876,14 @@
       <c r="C87" s="6">
         <v>40841.923611111109</v>
       </c>
-      <c r="D87" s="3"/>
-    </row>
-    <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D87" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E87" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>60</v>
       </c>
@@ -2783,9 +2893,14 @@
       <c r="C88" s="6">
         <v>41569.314583333333</v>
       </c>
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D88" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E88" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>106</v>
       </c>
@@ -2795,7 +2910,12 @@
       <c r="C89" s="6">
         <v>40934.828472222223</v>
       </c>
-      <c r="D89" s="3"/>
+      <c r="D89">
+        <v>1818656</v>
+      </c>
+      <c r="E89" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="90" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
@@ -2814,7 +2934,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>58</v>
       </c>
@@ -2824,7 +2944,12 @@
       <c r="C91" s="6">
         <v>41645.770138888889</v>
       </c>
-      <c r="D91" s="3"/>
+      <c r="D91" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E91" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="92" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
@@ -2867,7 +2992,7 @@
       </c>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>99</v>
       </c>
@@ -2877,9 +3002,14 @@
       <c r="C95" s="6">
         <v>41011.732638888891</v>
       </c>
-      <c r="D95" s="3"/>
-    </row>
-    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D95">
+        <v>1818656</v>
+      </c>
+      <c r="E95" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>111</v>
       </c>
@@ -2889,7 +3019,12 @@
       <c r="C96" s="6">
         <v>40891.341666666667</v>
       </c>
-      <c r="D96" s="3"/>
+      <c r="D96" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E96" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="97" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
@@ -2908,7 +3043,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>46</v>
       </c>
@@ -2942,7 +3077,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>103</v>
       </c>
@@ -2952,7 +3087,12 @@
       <c r="C100" s="6">
         <v>40954.956250000003</v>
       </c>
-      <c r="D100" s="3"/>
+      <c r="D100">
+        <v>1818656</v>
+      </c>
+      <c r="E100" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
@@ -3079,7 +3219,7 @@
       </c>
       <c r="D110" s="3"/>
     </row>
-    <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>88</v>
       </c>
@@ -3089,7 +3229,12 @@
       <c r="C111" s="6">
         <v>41107.82708333333</v>
       </c>
-      <c r="D111" s="3"/>
+      <c r="D111">
+        <v>1818656</v>
+      </c>
+      <c r="E111" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
@@ -3139,7 +3284,7 @@
       </c>
       <c r="D115" s="3"/>
     </row>
-    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>104</v>
       </c>
@@ -3149,7 +3294,12 @@
       <c r="C116" s="6">
         <v>40954.953472222223</v>
       </c>
-      <c r="D116" s="3"/>
+      <c r="D116">
+        <v>1818656</v>
+      </c>
+      <c r="E116" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
@@ -3163,7 +3313,7 @@
       </c>
       <c r="D117" s="3"/>
     </row>
-    <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>102</v>
       </c>
@@ -3173,7 +3323,12 @@
       <c r="C118" s="6">
         <v>40954.957638888889</v>
       </c>
-      <c r="D118" s="3"/>
+      <c r="D118">
+        <v>1818656</v>
+      </c>
+      <c r="E118" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
@@ -3187,7 +3342,7 @@
       </c>
       <c r="D119" s="3"/>
     </row>
-    <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>94</v>
       </c>
@@ -3197,7 +3352,12 @@
       <c r="C120" s="6">
         <v>41059.445833333331</v>
       </c>
-      <c r="D120" s="3"/>
+      <c r="D120">
+        <v>1818656</v>
+      </c>
+      <c r="E120" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
@@ -3211,7 +3371,7 @@
       </c>
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>169</v>
       </c>
@@ -3221,9 +3381,14 @@
       <c r="C122" s="6">
         <v>40288.902777777781</v>
       </c>
-      <c r="D122" s="3"/>
-    </row>
-    <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D122">
+        <v>1818656</v>
+      </c>
+      <c r="E122" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>49</v>
       </c>
@@ -3257,7 +3422,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>95</v>
       </c>
@@ -3332,7 +3497,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>115</v>
       </c>
@@ -3342,7 +3507,12 @@
       <c r="C130" s="6">
         <v>40886.088194444441</v>
       </c>
-      <c r="D130" s="3"/>
+      <c r="D130" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E130" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="131" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
@@ -3373,7 +3543,7 @@
       </c>
       <c r="D132" s="3"/>
     </row>
-    <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
         <v>79</v>
       </c>
@@ -3383,7 +3553,12 @@
       <c r="C133" s="6">
         <v>41199.607638888891</v>
       </c>
-      <c r="D133" s="3"/>
+      <c r="D133" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E133" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="134" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
@@ -3397,7 +3572,7 @@
       </c>
       <c r="D134" s="3"/>
     </row>
-    <row r="135" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>81</v>
       </c>
@@ -3407,7 +3582,12 @@
       <c r="C135" s="6">
         <v>41199.566666666666</v>
       </c>
-      <c r="D135" s="3"/>
+      <c r="D135" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E135" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="136" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
@@ -3503,7 +3683,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>73</v>
       </c>
@@ -3513,7 +3693,12 @@
       <c r="C143" s="6">
         <v>41271.527083333334</v>
       </c>
-      <c r="D143" s="3"/>
+      <c r="D143" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E143" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="144" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
@@ -3597,7 +3782,7 @@
       </c>
       <c r="D149" s="3"/>
     </row>
-    <row r="150" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>78</v>
       </c>
@@ -3607,9 +3792,14 @@
       <c r="C150" s="6">
         <v>41200.376388888886</v>
       </c>
-      <c r="D150" s="3"/>
-    </row>
-    <row r="151" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D150" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E150" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
         <v>86</v>
       </c>
@@ -3619,7 +3809,12 @@
       <c r="C151" s="6">
         <v>41107.863194444442</v>
       </c>
-      <c r="D151" s="3"/>
+      <c r="D151">
+        <v>1818656</v>
+      </c>
+      <c r="E151" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="152" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
@@ -3662,7 +3857,7 @@
       </c>
       <c r="D154" s="3"/>
     </row>
-    <row r="155" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
         <v>41</v>
       </c>
@@ -3708,7 +3903,7 @@
       </c>
       <c r="D157" s="3"/>
     </row>
-    <row r="158" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="5" t="s">
         <v>171</v>
       </c>
@@ -3720,7 +3915,7 @@
       </c>
       <c r="D158" s="3"/>
     </row>
-    <row r="159" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
         <v>50</v>
       </c>
@@ -3737,7 +3932,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="160" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
         <v>82</v>
       </c>
@@ -3747,9 +3942,14 @@
       <c r="C160" s="6">
         <v>41199.566666666666</v>
       </c>
-      <c r="D160" s="3"/>
-    </row>
-    <row r="161" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D160" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E160" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
         <v>77</v>
       </c>
@@ -3761,7 +3961,7 @@
       </c>
       <c r="D161" s="3"/>
     </row>
-    <row r="162" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="5" t="s">
         <v>153</v>
       </c>
@@ -3773,7 +3973,7 @@
       </c>
       <c r="D162" s="3"/>
     </row>
-    <row r="163" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
         <v>198</v>
       </c>
@@ -3785,7 +3985,7 @@
       </c>
       <c r="D163" s="3"/>
     </row>
-    <row r="164" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
         <v>83</v>
       </c>
@@ -3795,9 +3995,14 @@
       <c r="C164" s="6">
         <v>41169.689583333333</v>
       </c>
-      <c r="D164" s="3"/>
-    </row>
-    <row r="165" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D164">
+        <v>1818656</v>
+      </c>
+      <c r="E164" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
         <v>54</v>
       </c>
@@ -3809,7 +4014,7 @@
       </c>
       <c r="D165" s="3"/>
     </row>
-    <row r="166" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>42</v>
       </c>
@@ -3821,7 +4026,7 @@
       </c>
       <c r="D166" s="3"/>
     </row>
-    <row r="167" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>36</v>
       </c>
@@ -3833,7 +4038,7 @@
       </c>
       <c r="D167" s="3"/>
     </row>
-    <row r="168" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>37</v>
       </c>
@@ -3845,7 +4050,7 @@
       </c>
       <c r="D168" s="3"/>
     </row>
-    <row r="169" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>34</v>
       </c>
@@ -3857,7 +4062,7 @@
       </c>
       <c r="D169" s="3"/>
     </row>
-    <row r="170" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="5" t="s">
         <v>35</v>
       </c>
@@ -3869,7 +4074,7 @@
       </c>
       <c r="D170" s="3"/>
     </row>
-    <row r="171" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="5" t="s">
         <v>33</v>
       </c>
@@ -3881,7 +4086,7 @@
       </c>
       <c r="D171" s="3"/>
     </row>
-    <row r="172" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="5" t="s">
         <v>40</v>
       </c>
@@ -3893,7 +4098,7 @@
       </c>
       <c r="D172" s="3"/>
     </row>
-    <row r="173" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="5" t="s">
         <v>64</v>
       </c>
@@ -3903,9 +4108,14 @@
       <c r="C173" s="6">
         <v>41568.680555555555</v>
       </c>
-      <c r="D173" s="3"/>
-    </row>
-    <row r="174" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D173" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E173" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
         <v>85</v>
       </c>
@@ -3915,9 +4125,14 @@
       <c r="C174" s="6">
         <v>41107.863194444442</v>
       </c>
-      <c r="D174" s="3"/>
-    </row>
-    <row r="175" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D174">
+        <v>1818656</v>
+      </c>
+      <c r="E174" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
         <v>148</v>
       </c>
@@ -3929,7 +4144,7 @@
       </c>
       <c r="D175" s="3"/>
     </row>
-    <row r="176" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
         <v>155</v>
       </c>
@@ -3958,7 +4173,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="5" t="s">
         <v>71</v>
       </c>
@@ -3994,7 +4209,7 @@
       </c>
       <c r="D180" s="3"/>
     </row>
-    <row r="181" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="5" t="s">
         <v>45</v>
       </c>
@@ -4023,7 +4238,7 @@
       </c>
       <c r="D182" s="3"/>
     </row>
-    <row r="183" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
         <v>12</v>
       </c>
@@ -4040,7 +4255,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="184" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
         <v>44</v>
       </c>
@@ -4117,7 +4332,7 @@
       </c>
       <c r="D189" s="3"/>
     </row>
-    <row r="190" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="5" t="s">
         <v>91</v>
       </c>
@@ -4127,9 +4342,14 @@
       <c r="C190" s="6">
         <v>41074.51458333333</v>
       </c>
-      <c r="D190" s="3"/>
-    </row>
-    <row r="191" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D190">
+        <v>1818656</v>
+      </c>
+      <c r="E190" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="5" t="s">
         <v>90</v>
       </c>
@@ -4139,7 +4359,12 @@
       <c r="C191" s="6">
         <v>41074.51458333333</v>
       </c>
-      <c r="D191" s="3"/>
+      <c r="D191">
+        <v>1818656</v>
+      </c>
+      <c r="E191" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="192" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="5" t="s">
@@ -4204,7 +4429,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="5" t="s">
         <v>59</v>
       </c>
@@ -4214,9 +4439,14 @@
       <c r="C196" s="6">
         <v>41638.371527777781</v>
       </c>
-      <c r="D196" s="3"/>
-    </row>
-    <row r="197" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D196" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E196" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="5" t="s">
         <v>76</v>
       </c>
@@ -4226,7 +4456,12 @@
       <c r="C197" s="6">
         <v>41213.563194444447</v>
       </c>
-      <c r="D197" s="3"/>
+      <c r="D197" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E197" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="198" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="5" t="s">
@@ -4276,7 +4511,7 @@
       </c>
       <c r="D201" s="3"/>
     </row>
-    <row r="202" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="5" t="s">
         <v>113</v>
       </c>
@@ -4286,7 +4521,12 @@
       <c r="C202" s="6">
         <v>40891.311111111114</v>
       </c>
-      <c r="D202" s="3"/>
+      <c r="D202" s="3">
+        <v>1730821</v>
+      </c>
+      <c r="E202" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="203" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="5" t="s">
@@ -4300,7 +4540,7 @@
       </c>
       <c r="D203" s="3"/>
     </row>
-    <row r="204" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="5" t="s">
         <v>61</v>
       </c>
@@ -4310,9 +4550,14 @@
       <c r="C204" s="6">
         <v>41569.314583333333</v>
       </c>
-      <c r="D204" s="3"/>
-    </row>
-    <row r="205" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D204" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E204" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="5" t="s">
         <v>74</v>
       </c>
@@ -4322,9 +4567,14 @@
       <c r="C205" s="6">
         <v>41271.524305555555</v>
       </c>
-      <c r="D205" s="3"/>
-    </row>
-    <row r="206" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D205" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E205" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="5" t="s">
         <v>62</v>
       </c>
@@ -4334,7 +4584,12 @@
       <c r="C206" s="6">
         <v>41568.711111111108</v>
       </c>
-      <c r="D206" s="3"/>
+      <c r="D206" s="3">
+        <v>2116098</v>
+      </c>
+      <c r="E206" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="207" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="5" t="s">
@@ -4365,7 +4620,7 @@
       </c>
       <c r="D208" s="3"/>
     </row>
-    <row r="209" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="5" t="s">
         <v>43</v>
       </c>
@@ -4382,7 +4637,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="5" t="s">
         <v>84</v>
       </c>
@@ -4392,7 +4647,12 @@
       <c r="C210" s="6">
         <v>41107.863194444442</v>
       </c>
-      <c r="D210" s="3"/>
+      <c r="D210" s="9">
+        <v>1818656</v>
+      </c>
+      <c r="E210" s="9" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="211" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="5" t="s">
@@ -4447,7 +4707,7 @@
       </c>
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
         <v>93</v>
       </c>
@@ -4457,10 +4717,15 @@
       <c r="C215" s="6">
         <v>41059.445833333331</v>
       </c>
-      <c r="D215" s="3"/>
+      <c r="D215" s="9">
+        <v>1818656</v>
+      </c>
+      <c r="E215" s="9" t="s">
+        <v>221</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E215">
+  <autoFilter ref="A1:E215" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -4469,244 +4734,244 @@
     <sortCondition ref="A1:A215"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C1"/>
-    <hyperlink ref="A84" r:id="rId1" tooltip="Koly’s First At Bat" display="file:///324403888/settings"/>
-    <hyperlink ref="A213" r:id="rId2" tooltip="Who Eats Boogers?" display="file:///323991180/settings"/>
-    <hyperlink ref="A192" r:id="rId3" tooltip="Vanya Dices" display="file:///322646713/settings"/>
-    <hyperlink ref="A177" r:id="rId4" tooltip="The Longest Description" display="file:///314079416/settings"/>
-    <hyperlink ref="A77" r:id="rId5" tooltip="IMG_0003" display="file:///267306710/settings"/>
-    <hyperlink ref="A139" r:id="rId6" tooltip="rig inspection" display="file:///262221598/settings"/>
-    <hyperlink ref="A62" r:id="rId7" tooltip="Dunham Honor Choir - Christmas Songs 2016" display="file:///194259860/settings"/>
-    <hyperlink ref="A154" r:id="rId8" tooltip="St Lilian Academy Christmas Show (Older Kids) 1" display="file:///161715473/settings"/>
-    <hyperlink ref="A93" r:id="rId9" tooltip="Kolya's School Presentation" display="file:///160294977/settings"/>
-    <hyperlink ref="A182" r:id="rId10" tooltip="Toilet Singing" display="file:///160294908/settings"/>
-    <hyperlink ref="A211" r:id="rId11" tooltip="What Did Your Mom Tell You?" display="file:///159732659/settings"/>
-    <hyperlink ref="A201" r:id="rId12" tooltip="Vanya's Chapel Skit" display="file:///159721635/settings"/>
-    <hyperlink ref="A207" r:id="rId13" tooltip="Vanyaction" display="file:///159721594/settings"/>
-    <hyperlink ref="A47" r:id="rId14" tooltip="Dance Party" display="file:///159721583/settings"/>
-    <hyperlink ref="A214" r:id="rId15" tooltip="Who Had Fun at the Parade Tonight?" display="file:///159721579/settings"/>
-    <hyperlink ref="A55" r:id="rId16" tooltip="Double Sneaky Cats" display="file:///159721568/settings"/>
-    <hyperlink ref="A92" r:id="rId17" tooltip="Kolya's Knock Knock Joke" display="file:///159721557/settings"/>
-    <hyperlink ref="A97" r:id="rId18" tooltip="Lego Bulding" display="file:///159721543/settings"/>
-    <hyperlink ref="A137" r:id="rId19" tooltip="Really, Really, Really Hard Knock Life" display="file:///159721536/settings"/>
-    <hyperlink ref="A90" r:id="rId20" tooltip="Kolya is Making a Movie" display="file:///159721526/settings"/>
-    <hyperlink ref="A147" r:id="rId21" tooltip="Sk8ters" display="file:///159721516/settings"/>
-    <hyperlink ref="A61" r:id="rId22" tooltip="Dunham Halloween Carnival Day" display="file:///159721490/settings"/>
-    <hyperlink ref="A49" r:id="rId23" tooltip="Demo Day Kolya's Dance Class" display="file:///159721475/settings"/>
-    <hyperlink ref="A153" r:id="rId24" tooltip="Square Dancing" display="file:///159651315/settings"/>
-    <hyperlink ref="A59" r:id="rId25" tooltip="Drone Test - Stuck in Tree" display="file:///153437243/settings"/>
-    <hyperlink ref="A58" r:id="rId26" tooltip="Drone Flight - Goodwood Park" display="file:///153437208/settings"/>
-    <hyperlink ref="A142" r:id="rId27" tooltip="Sailing into Mandeville 2015-10-17" display="file:///142957004/settings"/>
-    <hyperlink ref="A194" r:id="rId28" tooltip="Vanya Opens Birthday Presents" display="file:///130789591/settings"/>
-    <hyperlink ref="A148" r:id="rId29" tooltip="Slow Damn Train" display="file:///130570160/settings"/>
-    <hyperlink ref="A101" r:id="rId30" tooltip="Louisiana Marathon Drone Mishap" display="file:///130486363/settings"/>
-    <hyperlink ref="A171" r:id="rId31" tooltip="Test Flight 5 - Westdale Middle School" display="file:///130363841/settings"/>
-    <hyperlink ref="A169" r:id="rId32" tooltip="Test Flight 3 - Westdale Middle School" display="file:///130363838/settings"/>
-    <hyperlink ref="A170" r:id="rId33" tooltip="Test Flight 4 - Westdale Middle School" display="file:///130363840/settings"/>
-    <hyperlink ref="A167" r:id="rId34" tooltip="Test Flight 1 - Westdale Middle School" display="file:///130363834/settings"/>
-    <hyperlink ref="A168" r:id="rId35" tooltip="Test Flight 2 - Westdale Middle School" display="file:///130363836/settings"/>
-    <hyperlink ref="A50" r:id="rId36" tooltip="Dinghy Captain Practice" display="file:///130363252/settings"/>
-    <hyperlink ref="A29" r:id="rId37" tooltip="Christmas Morning 2014" display="file:///130271126/settings"/>
-    <hyperlink ref="A172" r:id="rId38" tooltip="Test Flight at My House" display="file:///130265122/settings"/>
-    <hyperlink ref="A155" r:id="rId39" tooltip="St Lilian Academy Christmas Show 2014 (Big Kid Group)" display="file:///130263083/settings"/>
-    <hyperlink ref="A166" r:id="rId40" tooltip="Test Flight" display="file:///130253338/settings"/>
-    <hyperlink ref="A183" r:id="rId41" tooltip="Toilet Singing" display="file:///130251912/settings"/>
-    <hyperlink ref="A209" r:id="rId42" tooltip="Voodoo Dancing 2015" display="file:///130239757/settings"/>
-    <hyperlink ref="A184" r:id="rId43" tooltip="Trick or Treat Practice" display="file:///116100007/settings"/>
-    <hyperlink ref="A181" r:id="rId44" tooltip="Three Minutes Just the Other Day" display="file:///115911668/settings"/>
-    <hyperlink ref="A98" r:id="rId45" tooltip="Look at Sandra Dee" display="file:///115824161/settings"/>
-    <hyperlink ref="A76" r:id="rId46" tooltip="If You're Sailing With Me, Don't Be Afraid to Dance Bottomless" display="file:///99699615/settings"/>
-    <hyperlink ref="A67" r:id="rId47" tooltip="Exploring the wildlife at a secluded Florida anchorage." display="file:///99697885/settings"/>
-    <hyperlink ref="A123" r:id="rId48" tooltip="New Swimmer" display="file:///97777878/settings"/>
-    <hyperlink ref="A159" r:id="rId49" tooltip="Swim Kids" display="file:///97777879/settings"/>
-    <hyperlink ref="A80" r:id="rId50" tooltip="Jesus Camp Play" display="file:///97689396/settings"/>
-    <hyperlink ref="A48" r:id="rId51" tooltip="Dance Party" display="file:///93940290/settings"/>
-    <hyperlink ref="A40" r:id="rId52" tooltip="Creepiest Pop-Up Ad Ever" display="file:///93940292/settings"/>
-    <hyperlink ref="A81" r:id="rId53" tooltip="Just a Day on the Swings" display="file:///93937125/settings"/>
-    <hyperlink ref="A165" r:id="rId54" tooltip="Tedium in Column Highlighting" display="file:///93936938/settings"/>
-    <hyperlink ref="A57" r:id="rId55" tooltip="Driving the Train" display="file:///93936925/settings"/>
-    <hyperlink ref="A54" r:id="rId56" tooltip="Don't Get a Speeding Ticket, Lady" display="file:///93936926/settings"/>
-    <hyperlink ref="A82" r:id="rId57" tooltip="K's 3rd Birthday" display="file:///83546174/settings"/>
-    <hyperlink ref="A91" r:id="rId58" tooltip="Kolya School Xmas" display="file:///83545684/settings"/>
-    <hyperlink ref="A196" r:id="rId59" tooltip="Vanya School Xmas 2013" display="file:///82955738/settings"/>
-    <hyperlink ref="A88" r:id="rId60" tooltip="Kolya cut and paste crafts" display="file:///77496129/settings"/>
-    <hyperlink ref="A204" r:id="rId61" tooltip="Vanya's Spring Violin Recital" display="file:///77496130/settings"/>
-    <hyperlink ref="A206" r:id="rId62" tooltip="Vanya's Voice Recital - Spring 2012" display="file:///77451065/settings"/>
-    <hyperlink ref="A18" r:id="rId63" tooltip="Brother D-Day, Brother Flounder, Meet Brother Bluto" display="file:///77448013/settings"/>
-    <hyperlink ref="A173" r:id="rId64" tooltip="Testing the Really Big Slide at New Orleans City Park" display="file:///77447726/settings"/>
-    <hyperlink ref="A121" r:id="rId65" tooltip="MVI 0544" display="file:///77429020/settings"/>
-    <hyperlink ref="A19" r:id="rId66" tooltip="Brothers" display="file:///73741726/settings"/>
-    <hyperlink ref="A6" r:id="rId67" tooltip="At Anchor, Annapolis, MD" display="file:///73738599/settings"/>
-    <hyperlink ref="A46" r:id="rId68" tooltip="Dance Like There's No One Watching" display="file:///73423079/settings"/>
-    <hyperlink ref="A179" r:id="rId69" tooltip="This Cat Hates My Mom" display="file:///61238332/settings"/>
-    <hyperlink ref="A113" r:id="rId70" tooltip="Mardi Gras Indians 2013" display="file:///60428541/settings"/>
-    <hyperlink ref="A178" r:id="rId71" tooltip="The Most Inappropriate Birthday Card Ever Given to a Seven Year Old" display="file:///59033926/settings"/>
-    <hyperlink ref="A15" r:id="rId72" tooltip="Bounce Bounce Bounce" display="file:///56516060/settings"/>
-    <hyperlink ref="A143" r:id="rId73" tooltip="Shepherd #2" display="file:///56433496/settings"/>
-    <hyperlink ref="A205" r:id="rId74" tooltip="Vanya's Violin Recital" display="file:///56433307/settings"/>
-    <hyperlink ref="A85" r:id="rId75" tooltip="Kolya - Voodoo Fest 2012" display="file:///56432458/settings"/>
-    <hyperlink ref="A197" r:id="rId76" tooltip="Vanya Wins an Impossibly Hard Game" display="file:///52565728/settings"/>
-    <hyperlink ref="A161" r:id="rId77" tooltip="Tailgate Morning Peace" display="file:///52016381/settings"/>
-    <hyperlink ref="A150" r:id="rId78" tooltip="Solo Soccer" display="file:///51681142/settings"/>
-    <hyperlink ref="A133" r:id="rId79" tooltip="Polaris RZR" display="file:///51630449/settings"/>
-    <hyperlink ref="A38" r:id="rId80" tooltip="Couch Diving" display="file:///51629736/settings"/>
-    <hyperlink ref="A135" r:id="rId81" tooltip="Rain Boy" display="file:///51626169/settings"/>
-    <hyperlink ref="A160" r:id="rId82" tooltip="Swing!" display="file:///51626170/settings"/>
-    <hyperlink ref="A164" r:id="rId83" tooltip="Teaching a Baby Cards" display="file:///49635418/settings"/>
-    <hyperlink ref="A210" r:id="rId84" tooltip="Watching the Giraffe from the Animal Planet Lodge" display="file:///45942930/settings"/>
-    <hyperlink ref="A174" r:id="rId85" tooltip="The Boys Pick Up Leggos" display="file:///45942931/settings"/>
-    <hyperlink ref="A151" r:id="rId86" tooltip="Spill at the Schooner Wharf Bar" display="file:///45942929/settings"/>
-    <hyperlink ref="A112" r:id="rId87" tooltip="March with Pooh and Tigger" display="file:///45940964/settings"/>
-    <hyperlink ref="A111" r:id="rId88" tooltip="March of a Happy Kid" display="file:///45940962/settings"/>
-    <hyperlink ref="A23" r:id="rId89" tooltip="Carysfort Reef Lighthouse Starts Flashing for the Night" display="file:///45936859/settings"/>
-    <hyperlink ref="A191" r:id="rId90" tooltip="Vanya Dance Recital 2012 - The Tap" display="file:///44053153/settings"/>
-    <hyperlink ref="A190" r:id="rId91" tooltip="Vanya Dance Recital 2012 - The Ballet" display="file:///44053154/settings"/>
-    <hyperlink ref="A53" r:id="rId92" tooltip="Don't Get a Speeding Ticket, Guys" display="file:///43119210/settings"/>
-    <hyperlink ref="A215" r:id="rId93" tooltip="With the Next Selection of the 2031 NFL Draft, the Moon Colony Rockets Select Kolya Schultz" display="file:///43119207/settings"/>
-    <hyperlink ref="A120" r:id="rId94" tooltip="Moves" display="file:///43119208/settings"/>
-    <hyperlink ref="A125" r:id="rId95" tooltip="New Walker Practices Downhill and with Obsticles" display="file:///43119209/settings"/>
-    <hyperlink ref="A10" r:id="rId96" tooltip="Band in New Orleans" display="file:///41733084/settings"/>
-    <hyperlink ref="A28" r:id="rId97" tooltip="Chief Chocolate Face Calls His Tribe" display="file:///41028203/settings"/>
-    <hyperlink ref="A74" r:id="rId98" tooltip="Hot Dog Night" display="file:///40302576/settings"/>
-    <hyperlink ref="A95" r:id="rId99" tooltip="Lady Ga Ga Aboard" display="file:///40263629/settings"/>
-    <hyperlink ref="A25" r:id="rId100" tooltip="Cattle Stampede" display="file:///37671802/settings"/>
-    <hyperlink ref="A110" r:id="rId101" tooltip="Mamou Mardi Gras Finale" display="file:///37622541/settings"/>
-    <hyperlink ref="A118" r:id="rId102" tooltip="Monkey See - Monkey Do" display="file:///36880920/settings"/>
-    <hyperlink ref="A100" r:id="rId103" tooltip="Loose Tooth" display="file:///36880838/settings"/>
-    <hyperlink ref="A116" r:id="rId104" tooltip="Metallica Kid" display="file:///36880729/settings"/>
-    <hyperlink ref="A32" r:id="rId105" tooltip="Civil Engineering" display="file:///35770059/settings"/>
-    <hyperlink ref="A89" r:id="rId106" tooltip="Kolya Helps Vanya With Homework" display="file:///35727357/settings"/>
-    <hyperlink ref="A75" r:id="rId107" tooltip="Hotel Play, First Night with Kolya" display="file:///34011487/settings"/>
-    <hyperlink ref="A56" r:id="rId108" tooltip="Drive Up to the Orphanage for Gotcha Day" display="file:///34011051/settings"/>
-    <hyperlink ref="A13" r:id="rId109" tooltip="Bizzare Times in the Apple Foam Room" display="file:///33661817/settings"/>
-    <hyperlink ref="A17" r:id="rId110" tooltip="Breathing &quot;Massage&quot; for Kolya" display="file:///33661037/settings"/>
-    <hyperlink ref="A96" r:id="rId111" tooltip="Last Video of Us in the Orphange Play Room" display="file:///33660869/settings"/>
-    <hyperlink ref="A5" r:id="rId112" tooltip="Another Orphanage Visit Video" display="file:///33660585/settings"/>
-    <hyperlink ref="A202" r:id="rId113" tooltip="Vanya's First Snowballs" display="file:///33658914/settings"/>
-    <hyperlink ref="A208" r:id="rId114" tooltip="Violin Practice" display="file:///33583102/settings"/>
-    <hyperlink ref="A130" r:id="rId115" tooltip="Playing With Kolya on 2nd Trip" display="file:///33389238/settings"/>
-    <hyperlink ref="A73" r:id="rId116" tooltip="Homework in Yaroslavl" display="file:///33388431/settings"/>
-    <hyperlink ref="A94" r:id="rId117" tooltip="Kremlin Ceremony" display="file:///33191844/settings"/>
-    <hyperlink ref="A188" r:id="rId118" tooltip="V Doesn't Clean Up" display="file:///33189631/settings"/>
-    <hyperlink ref="A136" r:id="rId119" tooltip="Random Arrival to My Inbox" display="file:///31858617/settings"/>
-    <hyperlink ref="A203" r:id="rId120" tooltip="Vanya's Soccer Game 10/29/11" display="file:///31737600/settings"/>
-    <hyperlink ref="A87" r:id="rId121" tooltip="Kolya at his Orphanage 2" display="file:///31123796/settings"/>
-    <hyperlink ref="A86" r:id="rId122" tooltip="Kolya at His Orphanage" display="file:///31122896/settings"/>
-    <hyperlink ref="A189" r:id="rId123" tooltip="Vanya at Menche's" display="file:///31121908/settings"/>
-    <hyperlink ref="A4" r:id="rId124" tooltip="Annika Can't Work Up The Nerve" display="file:///26173972/settings"/>
-    <hyperlink ref="A66" r:id="rId125" tooltip="Evening Boat Tour of Lake George" display="file:///26167717/settings"/>
-    <hyperlink ref="A20" r:id="rId126" tooltip="Camilla Jumps Off Of Cliff" display="file:///26166164/settings"/>
-    <hyperlink ref="A42" r:id="rId127" tooltip="Crystal Jumps Off Cliff" display="file:///26165295/settings"/>
-    <hyperlink ref="A41" r:id="rId128" tooltip="Crystal Can't Work Up the Nerve" display="file:///26158320/settings"/>
-    <hyperlink ref="A79" r:id="rId129" tooltip="Jake Jumps Off Cliff" display="file:///26141891/settings"/>
-    <hyperlink ref="A12" r:id="rId130" tooltip="Ben Jumps Off Cliff" display="file:///26141649/settings"/>
-    <hyperlink ref="A33" r:id="rId131" tooltip="Clearing Brush" display="file:///26141630/settings"/>
-    <hyperlink ref="A157" r:id="rId132" tooltip="Sunset Over National Harbor" display="file:///25547002/settings"/>
-    <hyperlink ref="A149" r:id="rId133" tooltip="Slowest Sailboat Race Ever" display="file:///25220769/settings"/>
-    <hyperlink ref="A8" r:id="rId134" tooltip="Aunt Crystal Rides" display="file:///25220714/settings"/>
-    <hyperlink ref="A105" r:id="rId135" tooltip="Making Cookies - Part 2" display="file:///24952814/settings"/>
-    <hyperlink ref="A106" r:id="rId136" tooltip="Making Cookies - Part 3" display="file:///24951298/settings"/>
-    <hyperlink ref="A107" r:id="rId137" tooltip="Making Cookies - Part 4" display="file:///24950283/settings"/>
-    <hyperlink ref="A103" r:id="rId138" tooltip="Making Cookies - Finale" display="file:///24950053/settings"/>
-    <hyperlink ref="A104" r:id="rId139" tooltip="Making Cookies - Part 1" display="file:///24949664/settings"/>
-    <hyperlink ref="A186" r:id="rId140" tooltip="Trike-a-Thon 2011.  Trinity Episcopal Pre-K 4" display="file:///23046933/settings"/>
-    <hyperlink ref="A108" r:id="rId141" tooltip="Making Shoes for the Muses Parade" display="file:///23045562/settings"/>
-    <hyperlink ref="A11" r:id="rId142" tooltip="Ben and Vanya at the LSU Baseball Game" display="file:///23041025/settings"/>
-    <hyperlink ref="A63" r:id="rId143" tooltip="Easter Morning 2011" display="file:///22924722/settings"/>
-    <hyperlink ref="A200" r:id="rId144" tooltip="Vanya's Birthday 2011 - Presents at Home" display="file:///19814978/settings"/>
-    <hyperlink ref="A199" r:id="rId145" tooltip="Vanya's Birthday 2011 - Cake" display="file:///19813813/settings"/>
-    <hyperlink ref="A198" r:id="rId146" tooltip="Vanya's 2011 Birthday - Pinata" display="file:///19813606/settings"/>
-    <hyperlink ref="A114" r:id="rId147" tooltip="Meat Tenderizer" display="file:///18725569/settings"/>
-    <hyperlink ref="A175" r:id="rId148" tooltip="The Christmas God-Awful PVC Ferris Wheel" display="file:///18306263/settings"/>
-    <hyperlink ref="A31" r:id="rId149" tooltip="City Park Carousel" display="file:///17754806/settings"/>
-    <hyperlink ref="A134" r:id="rId150" tooltip="Pre-K4 Pilgrims and Indians" display="file:///17754725/settings"/>
-    <hyperlink ref="A60" r:id="rId151" tooltip="Drumming, Dancing" display="file:///17754074/settings"/>
-    <hyperlink ref="A185" r:id="rId152" tooltip="Trick Or Treating 2010" display="file:///17753896/settings"/>
-    <hyperlink ref="A162" r:id="rId153" tooltip="Tailgate Rainstorm" display="file:///17753317/settings"/>
-    <hyperlink ref="A117" r:id="rId154" tooltip="Mike the Tiger" display="file:///15808491/settings"/>
-    <hyperlink ref="A176" r:id="rId155" tooltip="The Lock" display="file:///14919393/settings"/>
-    <hyperlink ref="A115" r:id="rId156" tooltip="Mess" display="file:///14561249/settings"/>
-    <hyperlink ref="A132" r:id="rId157" tooltip="Playroom Cowboy" display="file:///14051534/settings"/>
-    <hyperlink ref="A146" r:id="rId158" tooltip="Singing on the Porch" display="file:///14050144/settings"/>
-    <hyperlink ref="A119" r:id="rId159" tooltip="More Play on the Beach" display="file:///14049203/settings"/>
-    <hyperlink ref="A141" r:id="rId160" tooltip="Run Away" display="file:///14049019/settings"/>
-    <hyperlink ref="A9" r:id="rId161" tooltip="Avalance on the Beach 8/2/2010" display="file:///14048853/settings"/>
-    <hyperlink ref="A126" r:id="rId162" tooltip="Nothing Happens in This One" display="file:///14040718/settings"/>
-    <hyperlink ref="A22" r:id="rId163" tooltip="Car Trip Fight?" display="file:///14040584/settings"/>
-    <hyperlink ref="A187" r:id="rId164" tooltip="Tubing - This One Is For the Conversation" display="file:///14020743/settings"/>
-    <hyperlink ref="A138" r:id="rId165" tooltip="Remote Control Boat" display="file:///14020664/settings"/>
-    <hyperlink ref="A152" r:id="rId166" tooltip="Splinter Removal" display="file:///14020270/settings"/>
-    <hyperlink ref="A68" r:id="rId167" tooltip="First T-Ball Game:  Fielding" display="file:///13045051/settings"/>
-    <hyperlink ref="A7" r:id="rId168" tooltip="At the French Quarter Festival" display="file:///11097122/settings"/>
-    <hyperlink ref="A122" r:id="rId169" tooltip="New Knives" display="file:///11096806/settings"/>
-    <hyperlink ref="A51" r:id="rId170" tooltip="Dinner With Lily" display="file:///10542756/settings"/>
-    <hyperlink ref="A158" r:id="rId171" tooltip="Superhero and Bartender University Just Added a Pre K Section" display="file:///10224361/settings"/>
-    <hyperlink ref="A212" r:id="rId172" tooltip="When the Saints Won the Superbowl" display="file:///9503551/settings"/>
-    <hyperlink ref="A140" r:id="rId173" tooltip="Royal Street after the Superbowl" display="file:///9500768/settings"/>
-    <hyperlink ref="A16" r:id="rId174" tooltip="Bourbon Street after the Superbowl" display="file:///9500417/settings"/>
-    <hyperlink ref="A3" r:id="rId175" tooltip="An Example of Why Sharples Makes Me Laugh" display="file:///9466435/settings"/>
-    <hyperlink ref="A37" r:id="rId176" tooltip="Coming out of Church Superbowl Sunday" display="file:///9406571/settings"/>
-    <hyperlink ref="A70" r:id="rId177" tooltip="French Quarter Before the Game on Superbowl Sunday" display="file:///9405742/settings"/>
-    <hyperlink ref="A102" r:id="rId178" tooltip="Making a Move about a Shark and a Dog" display="file:///9062297/settings"/>
-    <hyperlink ref="A36" r:id="rId179" tooltip="Close Your Eyes and Count to Four, the Sequel" display="file:///9062228/settings"/>
-    <hyperlink ref="A35" r:id="rId180" tooltip="Close Your Eyes and Count to Four" display="file:///9062169/settings"/>
-    <hyperlink ref="A71" r:id="rId181" tooltip="Game Day Drummer (NFC Championship Game Day)" display="file:///9014228/settings"/>
-    <hyperlink ref="A69" r:id="rId182" tooltip="Football with Batman" display="file:///9012706/settings"/>
-    <hyperlink ref="A78" r:id="rId183" tooltip="In the French Quarter on NFC Championship Gameday" display="file:///9012487/settings"/>
-    <hyperlink ref="A21" r:id="rId184" tooltip="Canal St. After the NFC Championship Game" display="file:///9011990/settings"/>
-    <hyperlink ref="A43" r:id="rId185" tooltip="Cutting the Grass in Maine" display="file:///6055193/settings"/>
-    <hyperlink ref="A127" r:id="rId186" tooltip="On the Beach" display="file:///6054747/settings"/>
-    <hyperlink ref="A26" r:id="rId187" tooltip="Chasing Birds in Boston" display="file:///6053533/settings"/>
-    <hyperlink ref="A34" r:id="rId188" tooltip="Clementine" display="file:///6053112/settings"/>
-    <hyperlink ref="A156" r:id="rId189" tooltip="Strongest Man Competition" display="file:///5658016/settings"/>
-    <hyperlink ref="A30" r:id="rId190" tooltip="Christmas Tree Decorating 2008" display="file:///2492003/settings"/>
-    <hyperlink ref="A2" r:id="rId191" tooltip="&quot;I Think He's Going To Be Worse Than Sam&quot;" display="file:///2491522/settings"/>
-    <hyperlink ref="A52" r:id="rId192" tooltip="Disobedient" display="file:///1434059/settings"/>
-    <hyperlink ref="A39" r:id="rId193" tooltip="Crazy Wild Beast" display="file:///1433978/settings"/>
-    <hyperlink ref="A45" r:id="rId194" tooltip="Dan Grooves" display="file:///1261871/settings"/>
-    <hyperlink ref="A145" r:id="rId195" tooltip="Singer in Thailand" display="file:///1261868/settings"/>
-    <hyperlink ref="A44" r:id="rId196" tooltip="Daisy Rolling in the Stink" display="file:///1261867/settings"/>
-    <hyperlink ref="A83" r:id="rId197" tooltip="Kitty Wars" display="file:///1229119/settings"/>
-    <hyperlink ref="A163" r:id="rId198" tooltip="Talking Cat !!?!" display="file:///1228780/settings"/>
-    <hyperlink ref="A131" r:id="rId199" tooltip="Playing with the Goat" display="file:///1203623/settings"/>
-    <hyperlink ref="A24" r:id="rId200" tooltip="Cat House/Goat Search" display="file:///1203621/settings"/>
-    <hyperlink ref="A124" r:id="rId201" tooltip="New Tricycle" display="file:///1119673/settings"/>
-    <hyperlink ref="A109" r:id="rId202" tooltip="Mama's Shoe" display="file:///1119670/settings"/>
-    <hyperlink ref="A64" r:id="rId203" tooltip="Enjoying Bad Country Music" display="file:///1109780/settings"/>
-    <hyperlink ref="A129" r:id="rId204" tooltip="Playing with Dog Toy and Camera" display="file:///1109706/settings"/>
-    <hyperlink ref="A99" r:id="rId205" tooltip="Looking for Maw Maw and Opa" display="file:///1109655/settings"/>
-    <hyperlink ref="A14" r:id="rId206" tooltip="Blossom Steals" display="file:///646905/settings"/>
-    <hyperlink ref="A180" r:id="rId207" tooltip="Three Lazy Beasts" display="file:///467464/settings"/>
-    <hyperlink ref="A27" r:id="rId208" tooltip="Chicken Dance Lemming" display="file:///467457/settings"/>
-    <hyperlink ref="A65" r:id="rId209" tooltip="Enjoying the Singing of the Whos from Whoville" display="file:///407910/settings"/>
-    <hyperlink ref="A195" r:id="rId210" tooltip="Vanya Plays Football, Chase, Etc." display="file:///406304/settings"/>
-    <hyperlink ref="A72" r:id="rId211" tooltip="Hit Me With That Pillow" display="file:///404193/settings"/>
-    <hyperlink ref="A144" r:id="rId212" tooltip="Show Me Your Belly" display="file:///404186/settings"/>
-    <hyperlink ref="A128" r:id="rId213" tooltip="Playing &quot;Here Comes That Old Bird&quot;" display="file:///404171/settings"/>
-    <hyperlink ref="A193" r:id="rId214" tooltip="Vanya getting hit by ball" display="file:///403997/settings"/>
+    <hyperlink ref="C1" display="Modified" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A84" r:id="rId1" tooltip="Koly’s First At Bat" display="file:///324403888/settings" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A213" r:id="rId2" tooltip="Who Eats Boogers?" display="file:///323991180/settings" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A192" r:id="rId3" tooltip="Vanya Dices" display="file:///322646713/settings" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A177" r:id="rId4" tooltip="The Longest Description" display="file:///314079416/settings" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A77" r:id="rId5" tooltip="IMG_0003" display="file:///267306710/settings" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A139" r:id="rId6" tooltip="rig inspection" display="file:///262221598/settings" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A62" r:id="rId7" tooltip="Dunham Honor Choir - Christmas Songs 2016" display="file:///194259860/settings" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A154" r:id="rId8" tooltip="St Lilian Academy Christmas Show (Older Kids) 1" display="file:///161715473/settings" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A93" r:id="rId9" tooltip="Kolya's School Presentation" display="file:///160294977/settings" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A182" r:id="rId10" tooltip="Toilet Singing" display="file:///160294908/settings" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A211" r:id="rId11" tooltip="What Did Your Mom Tell You?" display="file:///159732659/settings" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A201" r:id="rId12" tooltip="Vanya's Chapel Skit" display="file:///159721635/settings" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A207" r:id="rId13" tooltip="Vanyaction" display="file:///159721594/settings" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A47" r:id="rId14" tooltip="Dance Party" display="file:///159721583/settings" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A214" r:id="rId15" tooltip="Who Had Fun at the Parade Tonight?" display="file:///159721579/settings" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A55" r:id="rId16" tooltip="Double Sneaky Cats" display="file:///159721568/settings" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A92" r:id="rId17" tooltip="Kolya's Knock Knock Joke" display="file:///159721557/settings" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A97" r:id="rId18" tooltip="Lego Bulding" display="file:///159721543/settings" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A137" r:id="rId19" tooltip="Really, Really, Really Hard Knock Life" display="file:///159721536/settings" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A90" r:id="rId20" tooltip="Kolya is Making a Movie" display="file:///159721526/settings" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A147" r:id="rId21" tooltip="Sk8ters" display="file:///159721516/settings" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A61" r:id="rId22" tooltip="Dunham Halloween Carnival Day" display="file:///159721490/settings" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A49" r:id="rId23" tooltip="Demo Day Kolya's Dance Class" display="file:///159721475/settings" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A153" r:id="rId24" tooltip="Square Dancing" display="file:///159651315/settings" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A59" r:id="rId25" tooltip="Drone Test - Stuck in Tree" display="file:///153437243/settings" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A58" r:id="rId26" tooltip="Drone Flight - Goodwood Park" display="file:///153437208/settings" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A142" r:id="rId27" tooltip="Sailing into Mandeville 2015-10-17" display="file:///142957004/settings" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A194" r:id="rId28" tooltip="Vanya Opens Birthday Presents" display="file:///130789591/settings" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A148" r:id="rId29" tooltip="Slow Damn Train" display="file:///130570160/settings" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A101" r:id="rId30" tooltip="Louisiana Marathon Drone Mishap" display="file:///130486363/settings" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A171" r:id="rId31" tooltip="Test Flight 5 - Westdale Middle School" display="file:///130363841/settings" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A169" r:id="rId32" tooltip="Test Flight 3 - Westdale Middle School" display="file:///130363838/settings" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A170" r:id="rId33" tooltip="Test Flight 4 - Westdale Middle School" display="file:///130363840/settings" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A167" r:id="rId34" tooltip="Test Flight 1 - Westdale Middle School" display="file:///130363834/settings" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A168" r:id="rId35" tooltip="Test Flight 2 - Westdale Middle School" display="file:///130363836/settings" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A50" r:id="rId36" tooltip="Dinghy Captain Practice" display="file:///130363252/settings" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A29" r:id="rId37" tooltip="Christmas Morning 2014" display="file:///130271126/settings" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A172" r:id="rId38" tooltip="Test Flight at My House" display="file:///130265122/settings" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="A155" r:id="rId39" tooltip="St Lilian Academy Christmas Show 2014 (Big Kid Group)" display="file:///130263083/settings" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A166" r:id="rId40" tooltip="Test Flight" display="file:///130253338/settings" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="A183" r:id="rId41" tooltip="Toilet Singing" display="file:///130251912/settings" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A209" r:id="rId42" tooltip="Voodoo Dancing 2015" display="file:///130239757/settings" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="A184" r:id="rId43" tooltip="Trick or Treat Practice" display="file:///116100007/settings" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A181" r:id="rId44" tooltip="Three Minutes Just the Other Day" display="file:///115911668/settings" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A98" r:id="rId45" tooltip="Look at Sandra Dee" display="file:///115824161/settings" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A76" r:id="rId46" tooltip="If You're Sailing With Me, Don't Be Afraid to Dance Bottomless" display="file:///99699615/settings" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A67" r:id="rId47" tooltip="Exploring the wildlife at a secluded Florida anchorage." display="file:///99697885/settings" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A123" r:id="rId48" tooltip="New Swimmer" display="file:///97777878/settings" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="A159" r:id="rId49" tooltip="Swim Kids" display="file:///97777879/settings" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A80" r:id="rId50" tooltip="Jesus Camp Play" display="file:///97689396/settings" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A48" r:id="rId51" tooltip="Dance Party" display="file:///93940290/settings" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A40" r:id="rId52" tooltip="Creepiest Pop-Up Ad Ever" display="file:///93940292/settings" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="A81" r:id="rId53" tooltip="Just a Day on the Swings" display="file:///93937125/settings" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="A165" r:id="rId54" tooltip="Tedium in Column Highlighting" display="file:///93936938/settings" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="A57" r:id="rId55" tooltip="Driving the Train" display="file:///93936925/settings" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="A54" r:id="rId56" tooltip="Don't Get a Speeding Ticket, Lady" display="file:///93936926/settings" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="A82" r:id="rId57" tooltip="K's 3rd Birthday" display="file:///83546174/settings" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="A91" r:id="rId58" tooltip="Kolya School Xmas" display="file:///83545684/settings" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="A196" r:id="rId59" tooltip="Vanya School Xmas 2013" display="file:///82955738/settings" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="A88" r:id="rId60" tooltip="Kolya cut and paste crafts" display="file:///77496129/settings" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="A204" r:id="rId61" tooltip="Vanya's Spring Violin Recital" display="file:///77496130/settings" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="A206" r:id="rId62" tooltip="Vanya's Voice Recital - Spring 2012" display="file:///77451065/settings" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="A18" r:id="rId63" tooltip="Brother D-Day, Brother Flounder, Meet Brother Bluto" display="file:///77448013/settings" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="A173" r:id="rId64" tooltip="Testing the Really Big Slide at New Orleans City Park" display="file:///77447726/settings" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="A121" r:id="rId65" tooltip="MVI 0544" display="file:///77429020/settings" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="A19" r:id="rId66" tooltip="Brothers" display="file:///73741726/settings" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="A6" r:id="rId67" tooltip="At Anchor, Annapolis, MD" display="file:///73738599/settings" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="A46" r:id="rId68" tooltip="Dance Like There's No One Watching" display="file:///73423079/settings" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="A179" r:id="rId69" tooltip="This Cat Hates My Mom" display="file:///61238332/settings" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="A113" r:id="rId70" tooltip="Mardi Gras Indians 2013" display="file:///60428541/settings" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="A178" r:id="rId71" tooltip="The Most Inappropriate Birthday Card Ever Given to a Seven Year Old" display="file:///59033926/settings" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A15" r:id="rId72" tooltip="Bounce Bounce Bounce" display="file:///56516060/settings" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="A143" r:id="rId73" tooltip="Shepherd #2" display="file:///56433496/settings" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="A205" r:id="rId74" tooltip="Vanya's Violin Recital" display="file:///56433307/settings" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="A85" r:id="rId75" tooltip="Kolya - Voodoo Fest 2012" display="file:///56432458/settings" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="A197" r:id="rId76" tooltip="Vanya Wins an Impossibly Hard Game" display="file:///52565728/settings" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A161" r:id="rId77" tooltip="Tailgate Morning Peace" display="file:///52016381/settings" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="A150" r:id="rId78" tooltip="Solo Soccer" display="file:///51681142/settings" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="A133" r:id="rId79" tooltip="Polaris RZR" display="file:///51630449/settings" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="A38" r:id="rId80" tooltip="Couch Diving" display="file:///51629736/settings" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="A135" r:id="rId81" tooltip="Rain Boy" display="file:///51626169/settings" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="A160" r:id="rId82" tooltip="Swing!" display="file:///51626170/settings" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="A164" r:id="rId83" tooltip="Teaching a Baby Cards" display="file:///49635418/settings" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="A210" r:id="rId84" tooltip="Watching the Giraffe from the Animal Planet Lodge" display="file:///45942930/settings" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="A174" r:id="rId85" tooltip="The Boys Pick Up Leggos" display="file:///45942931/settings" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="A151" r:id="rId86" tooltip="Spill at the Schooner Wharf Bar" display="file:///45942929/settings" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A112" r:id="rId87" tooltip="March with Pooh and Tigger" display="file:///45940964/settings" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="A111" r:id="rId88" tooltip="March of a Happy Kid" display="file:///45940962/settings" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="A23" r:id="rId89" tooltip="Carysfort Reef Lighthouse Starts Flashing for the Night" display="file:///45936859/settings" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="A191" r:id="rId90" tooltip="Vanya Dance Recital 2012 - The Tap" display="file:///44053153/settings" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="A190" r:id="rId91" tooltip="Vanya Dance Recital 2012 - The Ballet" display="file:///44053154/settings" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="A53" r:id="rId92" tooltip="Don't Get a Speeding Ticket, Guys" display="file:///43119210/settings" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="A215" r:id="rId93" tooltip="With the Next Selection of the 2031 NFL Draft, the Moon Colony Rockets Select Kolya Schultz" display="file:///43119207/settings" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="A120" r:id="rId94" tooltip="Moves" display="file:///43119208/settings" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="A125" r:id="rId95" tooltip="New Walker Practices Downhill and with Obsticles" display="file:///43119209/settings" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="A10" r:id="rId96" tooltip="Band in New Orleans" display="file:///41733084/settings" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="A28" r:id="rId97" tooltip="Chief Chocolate Face Calls His Tribe" display="file:///41028203/settings" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="A74" r:id="rId98" tooltip="Hot Dog Night" display="file:///40302576/settings" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="A95" r:id="rId99" tooltip="Lady Ga Ga Aboard" display="file:///40263629/settings" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="A25" r:id="rId100" tooltip="Cattle Stampede" display="file:///37671802/settings" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="A110" r:id="rId101" tooltip="Mamou Mardi Gras Finale" display="file:///37622541/settings" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="A118" r:id="rId102" tooltip="Monkey See - Monkey Do" display="file:///36880920/settings" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="A100" r:id="rId103" tooltip="Loose Tooth" display="file:///36880838/settings" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="A116" r:id="rId104" tooltip="Metallica Kid" display="file:///36880729/settings" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="A32" r:id="rId105" tooltip="Civil Engineering" display="file:///35770059/settings" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="A89" r:id="rId106" tooltip="Kolya Helps Vanya With Homework" display="file:///35727357/settings" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="A75" r:id="rId107" tooltip="Hotel Play, First Night with Kolya" display="file:///34011487/settings" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="A56" r:id="rId108" tooltip="Drive Up to the Orphanage for Gotcha Day" display="file:///34011051/settings" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="A13" r:id="rId109" tooltip="Bizzare Times in the Apple Foam Room" display="file:///33661817/settings" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="A17" r:id="rId110" tooltip="Breathing &quot;Massage&quot; for Kolya" display="file:///33661037/settings" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="A96" r:id="rId111" tooltip="Last Video of Us in the Orphange Play Room" display="file:///33660869/settings" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="A5" r:id="rId112" tooltip="Another Orphanage Visit Video" display="file:///33660585/settings" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="A202" r:id="rId113" tooltip="Vanya's First Snowballs" display="file:///33658914/settings" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="A208" r:id="rId114" tooltip="Violin Practice" display="file:///33583102/settings" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="A130" r:id="rId115" tooltip="Playing With Kolya on 2nd Trip" display="file:///33389238/settings" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="A73" r:id="rId116" tooltip="Homework in Yaroslavl" display="file:///33388431/settings" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="A94" r:id="rId117" tooltip="Kremlin Ceremony" display="file:///33191844/settings" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="A188" r:id="rId118" tooltip="V Doesn't Clean Up" display="file:///33189631/settings" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="A136" r:id="rId119" tooltip="Random Arrival to My Inbox" display="file:///31858617/settings" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="A203" r:id="rId120" tooltip="Vanya's Soccer Game 10/29/11" display="file:///31737600/settings" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="A87" r:id="rId121" tooltip="Kolya at his Orphanage 2" display="file:///31123796/settings" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="A86" r:id="rId122" tooltip="Kolya at His Orphanage" display="file:///31122896/settings" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="A189" r:id="rId123" tooltip="Vanya at Menche's" display="file:///31121908/settings" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="A4" r:id="rId124" tooltip="Annika Can't Work Up The Nerve" display="file:///26173972/settings" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="A66" r:id="rId125" tooltip="Evening Boat Tour of Lake George" display="file:///26167717/settings" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="A20" r:id="rId126" tooltip="Camilla Jumps Off Of Cliff" display="file:///26166164/settings" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="A42" r:id="rId127" tooltip="Crystal Jumps Off Cliff" display="file:///26165295/settings" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="A41" r:id="rId128" tooltip="Crystal Can't Work Up the Nerve" display="file:///26158320/settings" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="A79" r:id="rId129" tooltip="Jake Jumps Off Cliff" display="file:///26141891/settings" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="A12" r:id="rId130" tooltip="Ben Jumps Off Cliff" display="file:///26141649/settings" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="A33" r:id="rId131" tooltip="Clearing Brush" display="file:///26141630/settings" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="A157" r:id="rId132" tooltip="Sunset Over National Harbor" display="file:///25547002/settings" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="A149" r:id="rId133" tooltip="Slowest Sailboat Race Ever" display="file:///25220769/settings" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="A8" r:id="rId134" tooltip="Aunt Crystal Rides" display="file:///25220714/settings" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="A105" r:id="rId135" tooltip="Making Cookies - Part 2" display="file:///24952814/settings" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="A106" r:id="rId136" tooltip="Making Cookies - Part 3" display="file:///24951298/settings" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="A107" r:id="rId137" tooltip="Making Cookies - Part 4" display="file:///24950283/settings" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="A103" r:id="rId138" tooltip="Making Cookies - Finale" display="file:///24950053/settings" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="A104" r:id="rId139" tooltip="Making Cookies - Part 1" display="file:///24949664/settings" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="A186" r:id="rId140" tooltip="Trike-a-Thon 2011.  Trinity Episcopal Pre-K 4" display="file:///23046933/settings" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="A108" r:id="rId141" tooltip="Making Shoes for the Muses Parade" display="file:///23045562/settings" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="A11" r:id="rId142" tooltip="Ben and Vanya at the LSU Baseball Game" display="file:///23041025/settings" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="A63" r:id="rId143" tooltip="Easter Morning 2011" display="file:///22924722/settings" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="A200" r:id="rId144" tooltip="Vanya's Birthday 2011 - Presents at Home" display="file:///19814978/settings" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="A199" r:id="rId145" tooltip="Vanya's Birthday 2011 - Cake" display="file:///19813813/settings" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="A198" r:id="rId146" tooltip="Vanya's 2011 Birthday - Pinata" display="file:///19813606/settings" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="A114" r:id="rId147" tooltip="Meat Tenderizer" display="file:///18725569/settings" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="A175" r:id="rId148" tooltip="The Christmas God-Awful PVC Ferris Wheel" display="file:///18306263/settings" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="A31" r:id="rId149" tooltip="City Park Carousel" display="file:///17754806/settings" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="A134" r:id="rId150" tooltip="Pre-K4 Pilgrims and Indians" display="file:///17754725/settings" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="A60" r:id="rId151" tooltip="Drumming, Dancing" display="file:///17754074/settings" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="A185" r:id="rId152" tooltip="Trick Or Treating 2010" display="file:///17753896/settings" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="A162" r:id="rId153" tooltip="Tailgate Rainstorm" display="file:///17753317/settings" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="A117" r:id="rId154" tooltip="Mike the Tiger" display="file:///15808491/settings" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="A176" r:id="rId155" tooltip="The Lock" display="file:///14919393/settings" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="A115" r:id="rId156" tooltip="Mess" display="file:///14561249/settings" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="A132" r:id="rId157" tooltip="Playroom Cowboy" display="file:///14051534/settings" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="A146" r:id="rId158" tooltip="Singing on the Porch" display="file:///14050144/settings" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="A119" r:id="rId159" tooltip="More Play on the Beach" display="file:///14049203/settings" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="A141" r:id="rId160" tooltip="Run Away" display="file:///14049019/settings" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="A9" r:id="rId161" tooltip="Avalance on the Beach 8/2/2010" display="file:///14048853/settings" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="A126" r:id="rId162" tooltip="Nothing Happens in This One" display="file:///14040718/settings" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="A22" r:id="rId163" tooltip="Car Trip Fight?" display="file:///14040584/settings" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="A187" r:id="rId164" tooltip="Tubing - This One Is For the Conversation" display="file:///14020743/settings" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="A138" r:id="rId165" tooltip="Remote Control Boat" display="file:///14020664/settings" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="A152" r:id="rId166" tooltip="Splinter Removal" display="file:///14020270/settings" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="A68" r:id="rId167" tooltip="First T-Ball Game:  Fielding" display="file:///13045051/settings" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="A7" r:id="rId168" tooltip="At the French Quarter Festival" display="file:///11097122/settings" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="A122" r:id="rId169" tooltip="New Knives" display="file:///11096806/settings" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="A51" r:id="rId170" tooltip="Dinner With Lily" display="file:///10542756/settings" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="A158" r:id="rId171" tooltip="Superhero and Bartender University Just Added a Pre K Section" display="file:///10224361/settings" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="A212" r:id="rId172" tooltip="When the Saints Won the Superbowl" display="file:///9503551/settings" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="A140" r:id="rId173" tooltip="Royal Street after the Superbowl" display="file:///9500768/settings" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="A16" r:id="rId174" tooltip="Bourbon Street after the Superbowl" display="file:///9500417/settings" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="A3" r:id="rId175" tooltip="An Example of Why Sharples Makes Me Laugh" display="file:///9466435/settings" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="A37" r:id="rId176" tooltip="Coming out of Church Superbowl Sunday" display="file:///9406571/settings" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="A70" r:id="rId177" tooltip="French Quarter Before the Game on Superbowl Sunday" display="file:///9405742/settings" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="A102" r:id="rId178" tooltip="Making a Move about a Shark and a Dog" display="file:///9062297/settings" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="A36" r:id="rId179" tooltip="Close Your Eyes and Count to Four, the Sequel" display="file:///9062228/settings" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="A35" r:id="rId180" tooltip="Close Your Eyes and Count to Four" display="file:///9062169/settings" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="A71" r:id="rId181" tooltip="Game Day Drummer (NFC Championship Game Day)" display="file:///9014228/settings" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="A69" r:id="rId182" tooltip="Football with Batman" display="file:///9012706/settings" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="A78" r:id="rId183" tooltip="In the French Quarter on NFC Championship Gameday" display="file:///9012487/settings" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="A21" r:id="rId184" tooltip="Canal St. After the NFC Championship Game" display="file:///9011990/settings" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="A43" r:id="rId185" tooltip="Cutting the Grass in Maine" display="file:///6055193/settings" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="A127" r:id="rId186" tooltip="On the Beach" display="file:///6054747/settings" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="A26" r:id="rId187" tooltip="Chasing Birds in Boston" display="file:///6053533/settings" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="A34" r:id="rId188" tooltip="Clementine" display="file:///6053112/settings" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="A156" r:id="rId189" tooltip="Strongest Man Competition" display="file:///5658016/settings" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="A30" r:id="rId190" tooltip="Christmas Tree Decorating 2008" display="file:///2492003/settings" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="A2" r:id="rId191" tooltip="&quot;I Think He's Going To Be Worse Than Sam&quot;" display="file:///2491522/settings" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="A52" r:id="rId192" tooltip="Disobedient" display="file:///1434059/settings" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="A39" r:id="rId193" tooltip="Crazy Wild Beast" display="file:///1433978/settings" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="A45" r:id="rId194" tooltip="Dan Grooves" display="file:///1261871/settings" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="A145" r:id="rId195" tooltip="Singer in Thailand" display="file:///1261868/settings" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="A44" r:id="rId196" tooltip="Daisy Rolling in the Stink" display="file:///1261867/settings" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="A83" r:id="rId197" tooltip="Kitty Wars" display="file:///1229119/settings" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="A163" r:id="rId198" tooltip="Talking Cat !!?!" display="file:///1228780/settings" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="A131" r:id="rId199" tooltip="Playing with the Goat" display="file:///1203623/settings" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="A24" r:id="rId200" tooltip="Cat House/Goat Search" display="file:///1203621/settings" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="A124" r:id="rId201" tooltip="New Tricycle" display="file:///1119673/settings" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="A109" r:id="rId202" tooltip="Mama's Shoe" display="file:///1119670/settings" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="A64" r:id="rId203" tooltip="Enjoying Bad Country Music" display="file:///1109780/settings" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="A129" r:id="rId204" tooltip="Playing with Dog Toy and Camera" display="file:///1109706/settings" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="A99" r:id="rId205" tooltip="Looking for Maw Maw and Opa" display="file:///1109655/settings" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="A14" r:id="rId206" tooltip="Blossom Steals" display="file:///646905/settings" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="A180" r:id="rId207" tooltip="Three Lazy Beasts" display="file:///467464/settings" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="A27" r:id="rId208" tooltip="Chicken Dance Lemming" display="file:///467457/settings" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="A65" r:id="rId209" tooltip="Enjoying the Singing of the Whos from Whoville" display="file:///407910/settings" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="A195" r:id="rId210" tooltip="Vanya Plays Football, Chase, Etc." display="file:///406304/settings" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="A72" r:id="rId211" tooltip="Hit Me With That Pillow" display="file:///404193/settings" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="A144" r:id="rId212" tooltip="Show Me Your Belly" display="file:///404186/settings" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="A128" r:id="rId213" tooltip="Playing &quot;Here Comes That Old Bird&quot;" display="file:///404171/settings" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="A193" r:id="rId214" tooltip="Vanya getting hit by ball" display="file:///403997/settings" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>219</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>220</v>
       </c>
     </row>
@@ -4774,15 +5039,42 @@
       <c r="A11">
         <v>2116098</v>
       </c>
+      <c r="B11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1818656</v>
       </c>
+      <c r="B12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1730821</v>
+      </c>
+      <c r="B13" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>